<commit_message>
guo tou dian li
</commit_message>
<xml_diff>
--- a/screensots/Daily.xlsx
+++ b/screensots/Daily.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>中信证券</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>1. 季线和月线有持续下跌趋势</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>国投电力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 非常接近L130 7.98
+2. 横盘整理</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -672,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -688,6 +697,7 @@
     <col min="8" max="8" width="20.25" customWidth="1"/>
     <col min="9" max="9" width="18.5" customWidth="1"/>
     <col min="10" max="10" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="22.5" x14ac:dyDescent="0.25">
@@ -719,7 +729,9 @@
       <c r="J1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="8"/>
+      <c r="K1" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:12" ht="74.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -753,6 +765,7 @@
       <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A3" s="12">
@@ -783,6 +796,9 @@
         <v>19</v>
       </c>
       <c r="J3" s="3"/>
+      <c r="K3" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
@@ -795,6 +811,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
+      <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>
@@ -807,6 +824,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
+      <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
@@ -819,6 +837,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
@@ -831,6 +850,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
@@ -843,6 +863,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
+      <c r="K8" s="4"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
@@ -855,6 +876,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
+      <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
@@ -867,6 +889,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
+      <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
@@ -879,6 +902,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
+      <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
@@ -891,6 +915,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
@@ -903,6 +928,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
+      <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
@@ -915,6 +941,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
@@ -927,6 +954,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
+      <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
@@ -939,8 +967,9 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="11"/>
       <c r="C17" s="3"/>
@@ -951,8 +980,9 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="11"/>
       <c r="C18" s="3"/>
@@ -963,8 +993,9 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="11"/>
       <c r="C19" s="3"/>
@@ -975,8 +1006,9 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="11"/>
       <c r="C20" s="3"/>
@@ -987,8 +1019,9 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="11"/>
       <c r="C21" s="3"/>
@@ -999,8 +1032,9 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="11"/>
       <c r="C22" s="3"/>
@@ -1011,8 +1045,9 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="B23" s="11"/>
       <c r="C23" s="3"/>
@@ -1023,8 +1058,9 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="11"/>
       <c r="C24" s="3"/>
@@ -1035,8 +1071,9 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="11"/>
       <c r="C25" s="3"/>
@@ -1047,8 +1084,9 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="B26" s="11"/>
       <c r="C26" s="3"/>
@@ -1059,22 +1097,23 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>

</xml_diff>